<commit_message>
FP6 - Running different detector / descriptor combinations and looking at the differences in TTC estimation
</commit_message>
<xml_diff>
--- a/results/3DObjectTracking_Results.xlsx
+++ b/results/3DObjectTracking_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenpower/Development/GitHub Projects/SensorFusion-Projects/SensorFusionND-3D-Object-Tracking/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188E5F0F-44FD-9848-8AE3-12F3B8C2E423}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E7AB1E-9472-8541-AA94-6C53EA5DEC6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9940" yWindow="6300" windowWidth="38840" windowHeight="17820" activeTab="2" xr2:uid="{669A409B-D193-1243-8032-91F302D11FB1}"/>
   </bookViews>
@@ -6639,7 +6639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BAF804-578D-8247-A7EA-6F6AE5995009}">
   <dimension ref="A2:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P50" sqref="P50"/>
     </sheetView>
   </sheetViews>

</xml_diff>